<commit_message>
Permitir reingreso de PEDIDO desde AGPE_CLEAN y PRIMERAS VISITAS; duplicados los valida el usuario
</commit_message>
<xml_diff>
--- a/data_clean/BDPCP.xlsx
+++ b/data_clean/BDPCP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hector.gaviria\Desktop\AGPE_AUTOMATION\data_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14A6C21-F3F0-423C-8449-766FE040EA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489CBB84-463D-4938-9C11-2AD1DBD07620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ADF04F22-24AD-40E2-B032-5F732E0990B4}"/>
   </bookViews>
@@ -990,9 +990,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1102,6 +1099,9 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1116,13 +1116,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56E5386C-8117-4BA7-BA48-92453B13939E}" name="Tabla4" displayName="Tabla4" ref="A1:D245" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56E5386C-8117-4BA7-BA48-92453B13939E}" name="Tabla4" displayName="Tabla4" ref="A1:D245" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:D245" xr:uid="{56E5386C-8117-4BA7-BA48-92453B13939E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F24790A3-435D-471A-B2C6-2755C4F5B43D}" name="PEDIDO" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A210EA58-7D38-4B8E-881F-C9C65666B19C}" name="PROMOTOR" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{852D57A2-2CBD-4406-B852-0BEB594B48E3}" name="CELULAR" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D6C705F6-2BBC-4B94-A814-F618396AFFA9}" name="POTENCIA AC [KW]" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F24790A3-435D-471A-B2C6-2755C4F5B43D}" name="PEDIDO" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A210EA58-7D38-4B8E-881F-C9C65666B19C}" name="PROMOTOR" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{852D57A2-2CBD-4406-B852-0BEB594B48E3}" name="CELULAR" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D6C705F6-2BBC-4B94-A814-F618396AFFA9}" name="POTENCIA AC [KW]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4891,7 +4891,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A245">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>